<commit_message>
click to order label for landing page and call to order if no landing page exist for an insert
</commit_message>
<xml_diff>
--- a/data/Dental_data.xlsx
+++ b/data/Dental_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andy\OneDrive\Desktop\Master Database\DentalLoupeInserts_Biolase\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andy\OneDrive\Desktop\DentalLoupeInserts\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3DFA372-B373-414B-BF22-4A96F494F53A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3ADD036C-41AF-4E86-BC97-9930AA8413FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{29F14E0B-5742-47C3-A3C8-7961C9D3ABD6}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{29F14E0B-5742-47C3-A3C8-7961C9D3ABD6}"/>
   </bookViews>
   <sheets>
     <sheet name="laser_info" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="994" uniqueCount="417">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1051" uniqueCount="430">
   <si>
     <t xml:space="preserve">Laser Mfg </t>
   </si>
@@ -916,11 +916,6 @@
     <t>Fair transmission of green light, lightweight and relatively inexpensive</t>
   </si>
   <si>
-    <t>190-450nm (OD 4), 655-665nm (OD 2), 
-730-1085nm (OD 5), 755nm (OD 7), 
-1064nm (OD 7), 9000-11000nm (OD 7)</t>
-  </si>
-  <si>
     <t>https://innovativeoptics.com/pi4-laser-glasses-frames/</t>
   </si>
   <si>
@@ -955,9 +950,6 @@
     <t>High VLT, lightweight and relatively inexpensive</t>
   </si>
   <si>
-    <t>9000-11000nm (OD 7)</t>
-  </si>
-  <si>
     <t>https://innovativeoptics.com/pi11-laser-glasses-frames/</t>
   </si>
   <si>
@@ -971,11 +963,6 @@
   </si>
   <si>
     <t>Moderate transmission of light across the visible spectrum, blocks near infrared, lightweight</t>
-  </si>
-  <si>
-    <t>1010-1090nm (OD7), 1064nm (OD10), 
-1650-2700nm (OD4), 2700-3000nm (OD5), 
-9000-11000nm (OD7)</t>
   </si>
   <si>
     <t>https://innovativeoptics.com/wp-content/uploads/2022/02/Pi19-laser-glasses.jpeg</t>
@@ -1043,15 +1030,6 @@
     <t>Low VLT, lightweight and relatively inexpensive</t>
   </si>
   <si>
-    <t>190-532nm (OD 7), 
-720-770nm (OD 7), 
-755nm (OD 8), 
-770-800nm (OD 6), 
-800-900nm (OD 5), 
-900-1077nm (OD 6), 
-9000-11000nm (OD 7)</t>
-  </si>
-  <si>
     <t>https://innovativeoptics.com/pi18-laser-glasses-frames/</t>
   </si>
   <si>
@@ -1082,10 +1060,295 @@
     <t>Pi8</t>
   </si>
   <si>
+    <t>https://innovativeoptics.com/pi8-laser-glasses-frames/</t>
+  </si>
+  <si>
+    <t>https://innovativeoptics.com/wp-content/uploads/2018/10/Pi8-laser-glasses.jpg</t>
+  </si>
+  <si>
+    <t>graphs/Pi8_plot.png</t>
+  </si>
+  <si>
+    <t>Pi5</t>
+  </si>
+  <si>
+    <t>Low VLT, lightweight and great for patients</t>
+  </si>
+  <si>
+    <t>190-470nm (OD 5), 600-800nm (OD 1), 800-1750nm (OD 5), 830-1700nm (OD 6), 840-1600nm (OD 7), 870-1140nm (OD 8), 9000-11000nm (OD 7)</t>
+  </si>
+  <si>
+    <t>https://innovativeoptics.com/pi5-laser-glasses-frames/</t>
+  </si>
+  <si>
+    <t>https://innovativeoptics.com/wp-content/uploads/2021/04/Pi5-laser-glasses-2.jpg</t>
+  </si>
+  <si>
+    <t>graphs/Pi5_plot.png</t>
+  </si>
+  <si>
+    <t>GiT7</t>
+  </si>
+  <si>
+    <t>430nm-500nm (OD 5), 500-515nm (OD 2), 515-532nm (OD 0.5), 655-1000nm (OD 5), 1000-1025nm (OD 6), 1025-1400nm (OD 7), 1400-2400nm (OD 5), 2770-10600nm (OD5)</t>
+  </si>
+  <si>
+    <t>https://innovativeoptics.com/git7-laser-glasses-frames/</t>
+  </si>
+  <si>
+    <t>https://innovativeoptics.com/wp-content/uploads/2021/12/GiT7-circle-lenses.jpg</t>
+  </si>
+  <si>
+    <t>graphs/GiT7_plot.png</t>
+  </si>
+  <si>
+    <t>Pi15</t>
+  </si>
+  <si>
+    <t>Low VLT, lightweight and broadly protective</t>
+  </si>
+  <si>
+    <t>IPL Shade 5
+300-1400nm (OD 1.5), 
+9000-11000nm (OD 7)</t>
+  </si>
+  <si>
+    <t>https://innovativeoptics.com/shade-5-ipl-glasses-frames/</t>
+  </si>
+  <si>
+    <t>https://innovativeoptics.com/wp-content/uploads/2019/11/8x2-IPL-Shade5.png</t>
+  </si>
+  <si>
+    <t>graphs/Pi15_plot.png</t>
+  </si>
+  <si>
+    <t>800-830nm (OD 5), 9000-11000nm (OD 7)</t>
+  </si>
+  <si>
+    <t>https://innovativeoptics.com/pi1-laser-glasses-frames/</t>
+  </si>
+  <si>
+    <t>https://innovativeoptics.com/wp-content/uploads/2018/04/pi1.jpg</t>
+  </si>
+  <si>
+    <t>graphs/Pi1_plot.png</t>
+  </si>
+  <si>
+    <t>Pi19</t>
+  </si>
+  <si>
+    <t>Grey, neutral density filters with above average VLT, made of lightweight materials to reduce fatigue</t>
+  </si>
+  <si>
+    <t>520-532nm (OD 0.49), 9000-11000nm (OD 7)</t>
+  </si>
+  <si>
+    <t>https://innovativeoptics.com/pi19-laser-glasses-frames/</t>
+  </si>
+  <si>
+    <t>graphs/Pi19_plot.png</t>
+  </si>
+  <si>
+    <t>Pi17</t>
+  </si>
+  <si>
+    <t>Green lenses with high VLT, made with lightweight materials to reduce fatigue</t>
+  </si>
+  <si>
+    <t>https://innovativeoptics.com/pi17-laser-glasses-frames/</t>
+  </si>
+  <si>
+    <t>https://innovativeoptics.com/wp-content/uploads/2021/12/Pi17-laser-glasses.jpg</t>
+  </si>
+  <si>
+    <t>graphs/Pi17_plot.png</t>
+  </si>
+  <si>
+    <t>Pi30</t>
+  </si>
+  <si>
+    <t>Violet-blue lens, made with lightweight materials to reduce fatigue</t>
+  </si>
+  <si>
+    <t>610-630nm(OD 5), 630-660nm (OD6), 660-705nm (OD 8)</t>
+  </si>
+  <si>
+    <t>graphs/Pi30_plot.png</t>
+  </si>
+  <si>
+    <t>PP19</t>
+  </si>
+  <si>
+    <t>graphs/PP19_plot.png</t>
+  </si>
+  <si>
+    <t>Argon 2</t>
+  </si>
+  <si>
+    <t>Traditional</t>
+  </si>
+  <si>
+    <t>ClariTi 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IVL </t>
+  </si>
+  <si>
+    <t>InfiniTi 2</t>
+  </si>
+  <si>
+    <t>Stellar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pi23 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">701.Pi23 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">757.Pi23 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Convergent </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Siro Blue Plus </t>
+  </si>
+  <si>
+    <t>655-665nm OD1, 960-985nm OD5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">50-19 (on the inside of the nose bridge) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">53-19 (on the inside of the nose bridge) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">55-19 (on the inside of the nose bridge) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">58-19 (on the inside of the nose bridge) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">49-19 (on the inside of the nose bridge) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">51-19 (on the inside of the nose bridge) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">54-19 (on the inside of the nose bridge) </t>
+  </si>
+  <si>
+    <t>54-22 (inside frame, upper left)</t>
+  </si>
+  <si>
+    <t>52-24 (inside frame, upper left)</t>
+  </si>
+  <si>
+    <t>52-22 (inside frame, upper left)</t>
+  </si>
+  <si>
+    <t>50-24 (inside frame, upper left)</t>
+  </si>
+  <si>
+    <t>50-22 (inside frame, upper left)</t>
+  </si>
+  <si>
+    <t>48-24 (inside frame, upper left)</t>
+  </si>
+  <si>
+    <t>48-22 (inside frame, upper left)</t>
+  </si>
+  <si>
+    <t>48-20 (inside frame, upper left)</t>
+  </si>
+  <si>
+    <t>46-24 (inside frame, upper left)</t>
+  </si>
+  <si>
+    <t>46-22 (inside frame, upper left)</t>
+  </si>
+  <si>
+    <t>46-20 (inside frame, upper left)</t>
+  </si>
+  <si>
+    <t>44-22 (inside frame, upper left)</t>
+  </si>
+  <si>
+    <t>42-22 (inside frame, upper left)</t>
+  </si>
+  <si>
+    <t>55-17 (inside frame, upper left)</t>
+  </si>
+  <si>
+    <t>56-18 (inside frame, upper left)</t>
+  </si>
+  <si>
+    <t>https://innovativeoptics.com/pi30-laser-glasses-frames/</t>
+  </si>
+  <si>
+    <t>https://innovativeoptics.com/pi22-laser-glasses-frames/</t>
+  </si>
+  <si>
+    <t>https://innovativeoptics.com/pi23-laser-glasses-frames/</t>
+  </si>
+  <si>
+    <t>810nm OD 5+/980nm  OD 5+</t>
+  </si>
+  <si>
+    <t>Rudy/Rydon Standard lens</t>
+  </si>
+  <si>
+    <t>Rudy/Rydon Deep B lens</t>
+  </si>
+  <si>
+    <t>200-455nm (OD 5), 650-665nm (OD 1), 725-800nm (OD 5), 800-955nm (OD 5), 955-1080nm (OD 6), 9000-11000nm (OD 7)</t>
+  </si>
+  <si>
+    <t>53-19 Victory Small (located on the nose bridge)</t>
+  </si>
+  <si>
+    <t>55-19 Victory Medium (located on the nose bridge)</t>
+  </si>
+  <si>
+    <t>57-19  Victory Large (located on the nose bridge)</t>
+  </si>
+  <si>
+    <t>IVR.R</t>
+  </si>
+  <si>
+    <t>200-455nm (OD 5), 
+650-665nm (OD 1), 
+725-800nm (OD 5), 
+800-955nm (OD 5), 
+955-1080nm (OD 6), 
+9000-11000nm (OD 7)</t>
+  </si>
+  <si>
+    <t>200-455nm (OD 5), 
+650-665nm(OD 1), 
+725-800nm (OD 5), 
+800-955nm (OD 5), 
+955-1080nm (OD 6), 
+9000-11000nm (OD 7)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Xenosys </t>
+  </si>
+  <si>
+    <t>Pi32</t>
+  </si>
+  <si>
+    <t>Blue LIght (400-470nm) </t>
+  </si>
+  <si>
+    <t>200-470nm (OD5), 630-685nm (OD3), 685-700nm (OD6), 700-730nm (OD 6), 730-1090nm (OD 7), 9000-11000nm (OD 7)</t>
+  </si>
+  <si>
     <r>
       <t xml:space="preserve">1010-1091nm (OD 5), 
 1020-1078nm (OD 6), 
-1030-1070nm (OD 7), 
+1030-1080nm (OD 7), 
 </t>
     </r>
     <r>
@@ -1099,266 +1362,53 @@
     </r>
   </si>
   <si>
-    <t>https://innovativeoptics.com/pi8-laser-glasses-frames/</t>
-  </si>
-  <si>
-    <t>https://innovativeoptics.com/wp-content/uploads/2018/10/Pi8-laser-glasses.jpg</t>
-  </si>
-  <si>
-    <t>graphs/Pi8_plot.png</t>
-  </si>
-  <si>
-    <t>Pi5</t>
-  </si>
-  <si>
-    <t>Low VLT, lightweight and great for patients</t>
-  </si>
-  <si>
-    <t>190-470nm (OD 5), 600-800nm (OD 1), 800-1750nm (OD 5), 830-1700nm (OD 6), 840-1600nm (OD 7), 870-1140nm (OD 8), 9000-11000nm (OD 7)</t>
-  </si>
-  <si>
-    <t>https://innovativeoptics.com/pi5-laser-glasses-frames/</t>
-  </si>
-  <si>
-    <t>https://innovativeoptics.com/wp-content/uploads/2021/04/Pi5-laser-glasses-2.jpg</t>
-  </si>
-  <si>
-    <t>graphs/Pi5_plot.png</t>
-  </si>
-  <si>
-    <t>GiT7</t>
-  </si>
-  <si>
-    <t>430nm-500nm (OD 5), 500-515nm (OD 2), 515-532nm (OD 0.5), 655-1000nm (OD 5), 1000-1025nm (OD 6), 1025-1400nm (OD 7), 1400-2400nm (OD 5), 2770-10600nm (OD5)</t>
-  </si>
-  <si>
-    <t>https://innovativeoptics.com/git7-laser-glasses-frames/</t>
-  </si>
-  <si>
-    <t>https://innovativeoptics.com/wp-content/uploads/2021/12/GiT7-circle-lenses.jpg</t>
-  </si>
-  <si>
-    <t>graphs/GiT7_plot.png</t>
-  </si>
-  <si>
-    <t>Pi15</t>
-  </si>
-  <si>
-    <t>Low VLT, lightweight and broadly protective</t>
-  </si>
-  <si>
-    <t>IPL Shade 5
-300-1400nm (OD 1.5), 
+    <t xml:space="preserve">
+IPAL-001-21-10</t>
+  </si>
+  <si>
+    <t>IPAX-001-21-04</t>
+  </si>
+  <si>
+    <t>IPHX-001-21-10</t>
+  </si>
+  <si>
+    <t>Triumph</t>
+  </si>
+  <si>
+    <t>Phantom</t>
+  </si>
+  <si>
+    <t>Elevate</t>
+  </si>
+  <si>
+    <t>Orascoptic Current Models</t>
+  </si>
+  <si>
+    <t>190-450nm (OD 4), 650-665nm (OD 2), 
+730-1085nm (OD 5), 755nm (OD 7), 
+1064nm (OD 7), 9000-11000nm (OD 7)</t>
+  </si>
+  <si>
+    <t>190-370 (OD 5),
 9000-11000nm (OD 7)</t>
   </si>
   <si>
-    <t>https://innovativeoptics.com/shade-5-ipl-glasses-frames/</t>
-  </si>
-  <si>
-    <t>https://innovativeoptics.com/wp-content/uploads/2019/11/8x2-IPL-Shade5.png</t>
-  </si>
-  <si>
-    <t>graphs/Pi15_plot.png</t>
-  </si>
-  <si>
-    <t>800-830nm (OD 5), 9000-11000nm (OD 7)</t>
-  </si>
-  <si>
-    <t>https://innovativeoptics.com/pi1-laser-glasses-frames/</t>
-  </si>
-  <si>
-    <t>https://innovativeoptics.com/wp-content/uploads/2018/04/pi1.jpg</t>
-  </si>
-  <si>
-    <t>graphs/Pi1_plot.png</t>
-  </si>
-  <si>
-    <t>Pi19</t>
-  </si>
-  <si>
-    <t>Grey, neutral density filters with above average VLT, made of lightweight materials to reduce fatigue</t>
-  </si>
-  <si>
-    <t>520-532nm (OD 0.49), 9000-11000nm (OD 7)</t>
-  </si>
-  <si>
-    <t>https://innovativeoptics.com/pi19-laser-glasses-frames/</t>
-  </si>
-  <si>
-    <t>graphs/Pi19_plot.png</t>
-  </si>
-  <si>
-    <t>Pi17</t>
-  </si>
-  <si>
-    <t>Green lenses with high VLT, made with lightweight materials to reduce fatigue</t>
-  </si>
-  <si>
-    <t>https://innovativeoptics.com/pi17-laser-glasses-frames/</t>
-  </si>
-  <si>
-    <t>https://innovativeoptics.com/wp-content/uploads/2021/12/Pi17-laser-glasses.jpg</t>
-  </si>
-  <si>
-    <t>graphs/Pi17_plot.png</t>
-  </si>
-  <si>
-    <t>Pi30</t>
-  </si>
-  <si>
-    <t>Violet-blue lens, made with lightweight materials to reduce fatigue</t>
-  </si>
-  <si>
-    <t>610-630nm(OD 5), 630-660nm (OD6), 660-705nm (OD 8)</t>
-  </si>
-  <si>
-    <t>graphs/Pi30_plot.png</t>
-  </si>
-  <si>
-    <t>PP19</t>
-  </si>
-  <si>
-    <t>graphs/PP19_plot.png</t>
-  </si>
-  <si>
-    <t>Argon 2</t>
-  </si>
-  <si>
-    <t>Traditional</t>
-  </si>
-  <si>
-    <t>ClariTi 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IVL </t>
-  </si>
-  <si>
-    <t>InfiniTi 2</t>
-  </si>
-  <si>
-    <t>Stellar</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pi23 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">701.Pi23 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">757.Pi23 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Convergent </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Siro Blue Plus </t>
-  </si>
-  <si>
-    <t>655-665nm OD1, 960-985nm OD5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">50-19 (on the inside of the nose bridge) </t>
-  </si>
-  <si>
-    <t xml:space="preserve">53-19 (on the inside of the nose bridge) </t>
-  </si>
-  <si>
-    <t xml:space="preserve">55-19 (on the inside of the nose bridge) </t>
-  </si>
-  <si>
-    <t xml:space="preserve">58-19 (on the inside of the nose bridge) </t>
-  </si>
-  <si>
-    <t xml:space="preserve">49-19 (on the inside of the nose bridge) </t>
-  </si>
-  <si>
-    <t xml:space="preserve">51-19 (on the inside of the nose bridge) </t>
-  </si>
-  <si>
-    <t xml:space="preserve">54-19 (on the inside of the nose bridge) </t>
-  </si>
-  <si>
-    <t>54-22 (inside frame, upper left)</t>
-  </si>
-  <si>
-    <t>52-24 (inside frame, upper left)</t>
-  </si>
-  <si>
-    <t>52-22 (inside frame, upper left)</t>
-  </si>
-  <si>
-    <t>50-24 (inside frame, upper left)</t>
-  </si>
-  <si>
-    <t>50-22 (inside frame, upper left)</t>
-  </si>
-  <si>
-    <t>48-24 (inside frame, upper left)</t>
-  </si>
-  <si>
-    <t>48-22 (inside frame, upper left)</t>
-  </si>
-  <si>
-    <t>48-20 (inside frame, upper left)</t>
-  </si>
-  <si>
-    <t>46-24 (inside frame, upper left)</t>
-  </si>
-  <si>
-    <t>46-22 (inside frame, upper left)</t>
-  </si>
-  <si>
-    <t>46-20 (inside frame, upper left)</t>
-  </si>
-  <si>
-    <t>44-22 (inside frame, upper left)</t>
-  </si>
-  <si>
-    <t>42-22 (inside frame, upper left)</t>
-  </si>
-  <si>
-    <t>55-17 (inside frame, upper left)</t>
-  </si>
-  <si>
-    <t>56-18 (inside frame, upper left)</t>
-  </si>
-  <si>
-    <t>200-455nm (OD 5), 
-630-670nm (OD 1), 
-725-800nm (OD 5), 
-800-955nm (OD 5), 
-955-1080nm (OD 6), 
+    <t>190-537nm (OD 8),
+650-670nm (OD 2),
+720-770nm (OD 7), 
+755nm (OD 8), 
+770-800nm (OD 6), 
+800-900nm (OD 5), 
+900-1077nm (OD 6), 
 9000-11000nm (OD 7)</t>
   </si>
   <si>
-    <t>https://innovativeoptics.com/pi30-laser-glasses-frames/</t>
-  </si>
-  <si>
-    <t>https://innovativeoptics.com/pi22-laser-glasses-frames/</t>
-  </si>
-  <si>
-    <t>https://innovativeoptics.com/pi23-laser-glasses-frames/</t>
-  </si>
-  <si>
-    <t>810nm OD 5+/980nm  OD 5+</t>
-  </si>
-  <si>
-    <t>Rudy/Rydon Standard lens</t>
-  </si>
-  <si>
-    <t>Rudy/Rydon Deep B lens</t>
-  </si>
-  <si>
-    <t>200-455nm (OD 5), 650-665nm (OD 1), 725-800nm (OD 5), 800-955nm (OD 5), 955-1080nm (OD 6), 9000-11000nm (OD 7)</t>
-  </si>
-  <si>
-    <t>53-19 Victory Small (located on the nose bridge)</t>
-  </si>
-  <si>
-    <t>55-19 Victory Medium (located on the nose bridge)</t>
-  </si>
-  <si>
-    <t>57-19  Victory Large (located on the nose bridge)</t>
+    <t>532nm (OD0.5)
+1010-1090nm (OD7)
+1064nm (OD10)
+1650-2700nm (OD4)
+2700-3000nm (OD5)
+9000-11000nm (OD7)</t>
   </si>
 </sst>
 </file>
@@ -1370,7 +1420,7 @@
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
     <numFmt numFmtId="164" formatCode="0\ %"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1434,6 +1484,17 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF1F1F1F"/>
+      <name val="Roboto"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -1461,7 +1522,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -1469,27 +1530,12 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1497,10 +1543,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1"/>
@@ -1520,6 +1562,14 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1835,23 +1885,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0F4191B-CE3C-4F0F-A124-77EB98865CC2}">
-  <dimension ref="A1:L40"/>
+  <dimension ref="A1:M40"/>
   <sheetViews>
-    <sheetView topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="18.44140625" customWidth="1"/>
     <col min="2" max="2" width="27.109375" customWidth="1"/>
-    <col min="3" max="3" width="21.6640625" customWidth="1"/>
+    <col min="3" max="3" width="50.44140625" customWidth="1"/>
     <col min="4" max="4" width="26.88671875" customWidth="1"/>
     <col min="5" max="10" width="14.77734375" customWidth="1"/>
-    <col min="12" max="12" width="14.44140625" customWidth="1"/>
+    <col min="11" max="11" width="103.77734375" customWidth="1"/>
+    <col min="12" max="13" width="98.109375" customWidth="1"/>
+    <col min="14" max="14" width="68.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1888,342 +1940,355 @@
       <c r="L1" s="1" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" ht="15.45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="M1" s="1" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" ht="15.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="C2" s="10" t="s">
         <v>12</v>
       </c>
       <c r="D2" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="13" t="s">
-        <v>378</v>
-      </c>
-      <c r="G2" s="13" t="s">
-        <v>379</v>
-      </c>
-      <c r="H2" s="13" t="s">
-        <v>380</v>
-      </c>
-      <c r="I2" s="14" t="s">
+      <c r="E2" s="11" t="s">
+        <v>373</v>
+      </c>
+      <c r="G2" s="11" t="s">
+        <v>374</v>
+      </c>
+      <c r="H2" s="11" t="s">
+        <v>375</v>
+      </c>
+      <c r="I2" s="12" t="s">
         <v>107</v>
       </c>
-      <c r="J2" s="15">
+      <c r="J2" s="13">
         <v>0.7</v>
       </c>
-      <c r="K2" s="5" t="s">
+      <c r="K2" s="20" t="s">
         <v>14</v>
       </c>
       <c r="L2" s="3"/>
-    </row>
-    <row r="3" spans="1:12" ht="15.45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="M2" s="3"/>
+    </row>
+    <row r="3" spans="1:13" ht="15.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="12" t="s">
+      <c r="C3" s="10" t="s">
         <v>12</v>
       </c>
       <c r="D3" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="13" t="s">
-        <v>378</v>
-      </c>
-      <c r="G3" s="13" t="s">
-        <v>379</v>
-      </c>
-      <c r="H3" s="13" t="s">
-        <v>380</v>
-      </c>
-      <c r="I3" s="14" t="s">
+      <c r="E3" s="11" t="s">
+        <v>373</v>
+      </c>
+      <c r="G3" s="11" t="s">
+        <v>374</v>
+      </c>
+      <c r="H3" s="11" t="s">
+        <v>375</v>
+      </c>
+      <c r="I3" s="12" t="s">
         <v>107</v>
       </c>
-      <c r="J3" s="15">
+      <c r="J3" s="13">
         <v>0.7</v>
       </c>
-      <c r="K3" s="5" t="s">
+      <c r="K3" s="21" t="s">
         <v>14</v>
       </c>
       <c r="L3" s="3"/>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M3" s="3"/>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="16" t="s">
+      <c r="B4" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="12" t="s">
+      <c r="C4" s="10" t="s">
         <v>18</v>
       </c>
       <c r="D4" t="s">
         <v>19</v>
       </c>
-      <c r="E4" s="13" t="s">
-        <v>378</v>
-      </c>
-      <c r="G4" s="13" t="s">
-        <v>379</v>
-      </c>
-      <c r="H4" s="13" t="s">
-        <v>380</v>
-      </c>
-      <c r="I4" s="14" t="s">
+      <c r="E4" s="11" t="s">
+        <v>373</v>
+      </c>
+      <c r="G4" s="11" t="s">
+        <v>374</v>
+      </c>
+      <c r="H4" s="11" t="s">
+        <v>375</v>
+      </c>
+      <c r="I4" s="12" t="s">
         <v>107</v>
       </c>
-      <c r="J4" s="15">
+      <c r="J4" s="13">
         <v>0.7</v>
       </c>
-      <c r="K4" s="5" t="s">
+      <c r="K4" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="L4" s="7"/>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="L4" s="5"/>
+      <c r="M4" s="5"/>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>20</v>
       </c>
-      <c r="B5" s="12" t="s">
+      <c r="B5" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="C5" s="12" t="s">
+      <c r="C5" s="10" t="s">
         <v>22</v>
       </c>
       <c r="D5" t="s">
         <v>23</v>
       </c>
-      <c r="E5" s="13" t="s">
-        <v>378</v>
-      </c>
-      <c r="G5" s="13" t="s">
-        <v>379</v>
-      </c>
-      <c r="H5" s="13" t="s">
-        <v>380</v>
-      </c>
-      <c r="I5" s="14" t="s">
+      <c r="E5" s="11" t="s">
+        <v>373</v>
+      </c>
+      <c r="G5" s="11" t="s">
+        <v>374</v>
+      </c>
+      <c r="H5" s="11" t="s">
+        <v>375</v>
+      </c>
+      <c r="I5" s="12" t="s">
         <v>107</v>
       </c>
-      <c r="J5" s="15">
+      <c r="J5" s="13">
         <v>0.7</v>
       </c>
-      <c r="K5" s="5" t="s">
+      <c r="K5" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="L5" s="7"/>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="L5" s="5"/>
+      <c r="M5" s="5"/>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="12" t="s">
+      <c r="B6" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="C6" s="12" t="s">
+      <c r="C6" s="10" t="s">
         <v>22</v>
       </c>
       <c r="D6" t="s">
         <v>23</v>
       </c>
-      <c r="E6" s="13" t="s">
-        <v>378</v>
-      </c>
-      <c r="G6" s="13" t="s">
-        <v>379</v>
-      </c>
-      <c r="H6" s="13" t="s">
-        <v>380</v>
-      </c>
-      <c r="I6" s="14" t="s">
+      <c r="E6" s="11" t="s">
+        <v>373</v>
+      </c>
+      <c r="G6" s="11" t="s">
+        <v>374</v>
+      </c>
+      <c r="H6" s="11" t="s">
+        <v>375</v>
+      </c>
+      <c r="I6" s="12" t="s">
         <v>107</v>
       </c>
-      <c r="J6" s="15">
+      <c r="J6" s="13">
         <v>0.7</v>
       </c>
-      <c r="K6" s="5" t="s">
+      <c r="K6" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="L6" s="7"/>
-    </row>
-    <row r="7" spans="1:12" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="L6" s="5"/>
+      <c r="M6" s="5"/>
+    </row>
+    <row r="7" spans="1:13" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="12" t="s">
+      <c r="B7" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="C7" s="12" t="s">
+      <c r="C7" s="10" t="s">
         <v>26</v>
       </c>
       <c r="D7" t="s">
         <v>19</v>
       </c>
-      <c r="E7" s="13" t="s">
-        <v>378</v>
-      </c>
-      <c r="G7" s="13" t="s">
-        <v>379</v>
-      </c>
-      <c r="H7" s="13" t="s">
-        <v>380</v>
-      </c>
-      <c r="I7" s="14" t="s">
+      <c r="E7" s="11" t="s">
+        <v>373</v>
+      </c>
+      <c r="G7" s="11" t="s">
+        <v>374</v>
+      </c>
+      <c r="H7" s="11" t="s">
+        <v>375</v>
+      </c>
+      <c r="I7" s="12" t="s">
         <v>107</v>
       </c>
-      <c r="J7" s="15">
+      <c r="J7" s="13">
         <v>0.7</v>
       </c>
-      <c r="K7" s="5" t="s">
+      <c r="K7" s="20" t="s">
         <v>14</v>
       </c>
       <c r="L7" s="3"/>
-    </row>
-    <row r="8" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="M7" s="3"/>
+    </row>
+    <row r="8" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="12" t="s">
+      <c r="B8" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="C8" s="12" t="s">
+      <c r="C8" s="10" t="s">
         <v>26</v>
       </c>
       <c r="D8" t="s">
         <v>19</v>
       </c>
-      <c r="E8" s="13" t="s">
-        <v>378</v>
-      </c>
-      <c r="G8" s="13" t="s">
-        <v>379</v>
-      </c>
-      <c r="H8" s="13" t="s">
-        <v>380</v>
-      </c>
-      <c r="I8" s="14" t="s">
+      <c r="E8" s="11" t="s">
+        <v>373</v>
+      </c>
+      <c r="G8" s="11" t="s">
+        <v>374</v>
+      </c>
+      <c r="H8" s="11" t="s">
+        <v>375</v>
+      </c>
+      <c r="I8" s="12" t="s">
         <v>107</v>
       </c>
-      <c r="J8" s="15">
+      <c r="J8" s="13">
         <v>0.7</v>
       </c>
-      <c r="K8" s="5" t="s">
+      <c r="K8" s="20" t="s">
         <v>14</v>
       </c>
       <c r="L8" s="3"/>
-    </row>
-    <row r="9" spans="1:12" ht="13.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="M8" s="3"/>
+    </row>
+    <row r="9" spans="1:13" ht="13.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>20</v>
       </c>
-      <c r="B9" s="12" t="s">
+      <c r="B9" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="C9" s="12" t="s">
+      <c r="C9" s="10" t="s">
         <v>26</v>
       </c>
       <c r="D9" t="s">
         <v>19</v>
       </c>
-      <c r="E9" s="13" t="s">
-        <v>378</v>
-      </c>
-      <c r="G9" s="13" t="s">
-        <v>379</v>
-      </c>
-      <c r="H9" s="13" t="s">
-        <v>380</v>
-      </c>
-      <c r="I9" s="14" t="s">
+      <c r="E9" s="11" t="s">
+        <v>373</v>
+      </c>
+      <c r="G9" s="11" t="s">
+        <v>374</v>
+      </c>
+      <c r="H9" s="11" t="s">
+        <v>375</v>
+      </c>
+      <c r="I9" s="12" t="s">
         <v>107</v>
       </c>
-      <c r="J9" s="15">
+      <c r="J9" s="13">
         <v>0.7</v>
       </c>
-      <c r="K9" s="5" t="s">
+      <c r="K9" s="20" t="s">
         <v>14</v>
       </c>
       <c r="L9" s="3"/>
-    </row>
-    <row r="10" spans="1:12" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="M9" s="3"/>
+    </row>
+    <row r="10" spans="1:13" ht="13.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>20</v>
       </c>
-      <c r="B10" s="12" t="s">
+      <c r="B10" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="C10" s="12" t="s">
+      <c r="C10" s="10" t="s">
         <v>26</v>
       </c>
       <c r="D10" t="s">
         <v>19</v>
       </c>
-      <c r="E10" s="13" t="s">
-        <v>378</v>
-      </c>
-      <c r="G10" s="13" t="s">
-        <v>379</v>
-      </c>
-      <c r="H10" s="13" t="s">
-        <v>380</v>
-      </c>
-      <c r="I10" s="14" t="s">
+      <c r="E10" s="11" t="s">
+        <v>373</v>
+      </c>
+      <c r="G10" s="11" t="s">
+        <v>374</v>
+      </c>
+      <c r="H10" s="11" t="s">
+        <v>375</v>
+      </c>
+      <c r="I10" s="12" t="s">
         <v>107</v>
       </c>
-      <c r="J10" s="15">
+      <c r="J10" s="13">
         <v>0.7</v>
       </c>
-      <c r="K10" s="5" t="s">
+      <c r="K10" s="20" t="s">
         <v>14</v>
       </c>
       <c r="L10" s="3"/>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M10" s="3"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>30</v>
       </c>
-      <c r="B11" s="17" t="s">
+      <c r="B11" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="C11" s="12" t="s">
+      <c r="C11" s="10" t="s">
         <v>18</v>
       </c>
       <c r="D11" t="s">
         <v>32</v>
       </c>
-      <c r="E11" s="13" t="s">
-        <v>378</v>
-      </c>
-      <c r="G11" s="13" t="s">
-        <v>379</v>
-      </c>
-      <c r="H11" s="13" t="s">
-        <v>380</v>
-      </c>
-      <c r="I11" s="14" t="s">
+      <c r="E11" s="11" t="s">
+        <v>373</v>
+      </c>
+      <c r="G11" s="11" t="s">
+        <v>374</v>
+      </c>
+      <c r="H11" s="11" t="s">
+        <v>375</v>
+      </c>
+      <c r="I11" s="12" t="s">
         <v>107</v>
       </c>
-      <c r="J11" s="15">
+      <c r="J11" s="13">
         <v>0.7</v>
       </c>
-      <c r="K11" s="5" t="s">
+      <c r="K11" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="L11" s="7"/>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="L11" s="5"/>
+      <c r="M11" s="5"/>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>50</v>
       </c>
-      <c r="B12" s="6" t="s">
+      <c r="B12" s="4" t="s">
         <v>100</v>
       </c>
       <c r="C12" t="s">
@@ -2235,922 +2300,953 @@
       <c r="E12" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="G12" s="14" t="s">
+      <c r="G12" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="H12" s="14" t="s">
+      <c r="H12" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="I12" s="14" t="s">
+      <c r="I12" s="12" t="s">
         <v>107</v>
       </c>
-      <c r="J12" s="15">
+      <c r="J12" s="13">
         <v>0.7</v>
       </c>
-      <c r="K12" s="5" t="s">
+      <c r="K12" s="20" t="s">
         <v>40</v>
       </c>
-      <c r="L12" s="7"/>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="L12" s="5"/>
+      <c r="M12" s="5"/>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>33</v>
       </c>
-      <c r="B13" s="12" t="s">
+      <c r="B13" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="C13" s="12" t="s">
+      <c r="C13" s="10" t="s">
         <v>35</v>
       </c>
       <c r="D13" t="s">
         <v>36</v>
       </c>
-      <c r="E13" s="14" t="s">
+      <c r="E13" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="G13" s="14" t="s">
+      <c r="G13" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="H13" s="14" t="s">
+      <c r="H13" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="I13" s="14" t="s">
+      <c r="I13" s="12" t="s">
         <v>107</v>
       </c>
-      <c r="J13" s="15">
+      <c r="J13" s="13">
         <v>0.7</v>
       </c>
-      <c r="K13" s="5" t="s">
+      <c r="K13" s="20" t="s">
         <v>40</v>
       </c>
-      <c r="L13" s="7"/>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="L13" s="5"/>
+      <c r="M13" s="5"/>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>33</v>
       </c>
-      <c r="B14" s="12" t="s">
+      <c r="B14" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="C14" s="12" t="s">
+      <c r="C14" s="10" t="s">
         <v>35</v>
       </c>
       <c r="D14" t="s">
         <v>36</v>
       </c>
-      <c r="E14" s="14" t="s">
+      <c r="E14" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="G14" s="14" t="s">
+      <c r="G14" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="H14" s="14" t="s">
+      <c r="H14" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="I14" s="14" t="s">
+      <c r="I14" s="12" t="s">
         <v>107</v>
       </c>
-      <c r="J14" s="15">
+      <c r="J14" s="13">
         <v>0.7</v>
       </c>
-      <c r="K14" s="5" t="s">
+      <c r="K14" s="20" t="s">
         <v>40</v>
       </c>
-      <c r="L14" s="7"/>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="L14" s="5"/>
+      <c r="M14" s="5"/>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>33</v>
       </c>
-      <c r="B15" s="12" t="s">
+      <c r="B15" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="C15" s="12" t="s">
+      <c r="C15" s="10" t="s">
         <v>35</v>
       </c>
       <c r="D15" t="s">
         <v>36</v>
       </c>
-      <c r="E15" s="14" t="s">
+      <c r="E15" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="G15" s="14" t="s">
+      <c r="G15" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="H15" s="14" t="s">
+      <c r="H15" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="I15" s="14" t="s">
+      <c r="I15" s="12" t="s">
         <v>107</v>
       </c>
-      <c r="J15" s="15">
+      <c r="J15" s="13">
         <v>0.7</v>
       </c>
-      <c r="K15" s="5" t="s">
+      <c r="K15" s="20" t="s">
         <v>40</v>
       </c>
-      <c r="L15" s="7"/>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="L15" s="5"/>
+      <c r="M15" s="5"/>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>43</v>
       </c>
-      <c r="B16" s="12" t="s">
+      <c r="B16" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="C16" s="12" t="s">
+      <c r="C16" s="10" t="s">
         <v>45</v>
       </c>
       <c r="D16" t="s">
         <v>36</v>
       </c>
-      <c r="E16" s="14" t="s">
+      <c r="E16" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="G16" s="14" t="s">
+      <c r="G16" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="H16" s="14" t="s">
+      <c r="H16" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="I16" s="14" t="s">
+      <c r="I16" s="12" t="s">
         <v>107</v>
       </c>
-      <c r="J16" s="15">
+      <c r="J16" s="13">
         <v>0.7</v>
       </c>
-      <c r="K16" s="5" t="s">
+      <c r="K16" s="20" t="s">
         <v>40</v>
       </c>
-      <c r="L16" s="7"/>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="L16" s="5"/>
+      <c r="M16" s="5"/>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>46</v>
       </c>
       <c r="B17" t="s">
         <v>47</v>
       </c>
-      <c r="C17" s="12" t="s">
+      <c r="C17" s="10" t="s">
         <v>45</v>
       </c>
       <c r="D17" t="s">
         <v>36</v>
       </c>
-      <c r="E17" s="14" t="s">
+      <c r="E17" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="G17" s="14" t="s">
+      <c r="G17" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="H17" s="14" t="s">
+      <c r="H17" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="I17" s="14" t="s">
+      <c r="I17" s="12" t="s">
         <v>107</v>
       </c>
-      <c r="J17" s="15">
+      <c r="J17" s="13">
         <v>0.7</v>
       </c>
-      <c r="K17" s="5" t="s">
+      <c r="K17" s="20" t="s">
         <v>40</v>
       </c>
-      <c r="L17" s="7"/>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="L17" s="5"/>
+      <c r="M17" s="5"/>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>48</v>
       </c>
       <c r="B18" t="s">
         <v>48</v>
       </c>
-      <c r="C18" s="12" t="s">
+      <c r="C18" s="10" t="s">
         <v>49</v>
       </c>
       <c r="D18" t="s">
         <v>36</v>
       </c>
-      <c r="E18" s="14" t="s">
+      <c r="E18" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="G18" s="14" t="s">
+      <c r="G18" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="H18" s="14" t="s">
+      <c r="H18" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="I18" s="14" t="s">
+      <c r="I18" s="12" t="s">
         <v>107</v>
       </c>
-      <c r="J18" s="15">
+      <c r="J18" s="13">
         <v>0.7</v>
       </c>
-      <c r="K18" s="5" t="s">
+      <c r="K18" s="20" t="s">
         <v>40</v>
       </c>
-      <c r="L18" s="7"/>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="L18" s="5"/>
+      <c r="M18" s="5"/>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>50</v>
       </c>
-      <c r="B19" s="12" t="s">
+      <c r="B19" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="C19" s="12" t="s">
+      <c r="C19" s="10" t="s">
         <v>45</v>
       </c>
       <c r="D19" t="s">
         <v>36</v>
       </c>
-      <c r="E19" s="14" t="s">
+      <c r="E19" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="G19" s="14" t="s">
+      <c r="G19" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="H19" s="14" t="s">
+      <c r="H19" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="I19" s="14" t="s">
+      <c r="I19" s="12" t="s">
         <v>107</v>
       </c>
-      <c r="J19" s="15">
+      <c r="J19" s="13">
         <v>0.7</v>
       </c>
-      <c r="K19" s="5" t="s">
+      <c r="K19" s="20" t="s">
         <v>40</v>
       </c>
-      <c r="L19" s="7"/>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="L19" s="5"/>
+      <c r="M19" s="5"/>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>52</v>
       </c>
-      <c r="B20" s="14" t="s">
+      <c r="B20" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="C20" s="12" t="s">
+      <c r="C20" s="10" t="s">
         <v>54</v>
       </c>
       <c r="D20" t="s">
         <v>36</v>
       </c>
-      <c r="E20" s="14" t="s">
+      <c r="E20" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="G20" s="14" t="s">
+      <c r="G20" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="H20" s="14" t="s">
+      <c r="H20" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="I20" s="14" t="s">
+      <c r="I20" s="12" t="s">
         <v>107</v>
       </c>
-      <c r="J20" s="15">
+      <c r="J20" s="13">
         <v>0.7</v>
       </c>
-      <c r="K20" s="5" t="s">
+      <c r="K20" s="20" t="s">
         <v>40</v>
       </c>
-      <c r="L20" s="7"/>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="L20" s="5"/>
+      <c r="M20" s="5"/>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>52</v>
       </c>
-      <c r="B21" s="14" t="s">
+      <c r="B21" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="C21" s="12" t="s">
+      <c r="C21" s="10" t="s">
         <v>56</v>
       </c>
       <c r="D21" t="s">
         <v>36</v>
       </c>
-      <c r="E21" s="14" t="s">
+      <c r="E21" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="G21" s="14" t="s">
+      <c r="G21" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="H21" s="14" t="s">
+      <c r="H21" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="I21" s="14" t="s">
+      <c r="I21" s="12" t="s">
         <v>107</v>
       </c>
-      <c r="J21" s="15">
+      <c r="J21" s="13">
         <v>0.7</v>
       </c>
-      <c r="K21" s="5" t="s">
+      <c r="K21" s="20" t="s">
         <v>40</v>
       </c>
-      <c r="L21" s="7"/>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="L21" s="5"/>
+      <c r="M21" s="5"/>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>52</v>
       </c>
-      <c r="B22" s="14" t="s">
+      <c r="B22" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="C22" s="12" t="s">
+      <c r="C22" s="10" t="s">
         <v>54</v>
       </c>
       <c r="D22" t="s">
         <v>36</v>
       </c>
-      <c r="E22" s="14" t="s">
+      <c r="E22" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="G22" s="14" t="s">
+      <c r="G22" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="H22" s="14" t="s">
+      <c r="H22" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="I22" s="14" t="s">
+      <c r="I22" s="12" t="s">
         <v>107</v>
       </c>
-      <c r="J22" s="15">
+      <c r="J22" s="13">
         <v>0.7</v>
       </c>
-      <c r="K22" s="5" t="s">
+      <c r="K22" s="20" t="s">
         <v>40</v>
       </c>
-      <c r="L22" s="7"/>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="L22" s="5"/>
+      <c r="M22" s="5"/>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>58</v>
       </c>
       <c r="B23" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="C23" s="12" t="s">
-        <v>410</v>
+      <c r="C23" s="10" t="s">
+        <v>404</v>
       </c>
       <c r="D23" t="s">
         <v>36</v>
       </c>
-      <c r="E23" s="14" t="s">
+      <c r="E23" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="G23" s="14" t="s">
+      <c r="G23" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="H23" s="14" t="s">
+      <c r="H23" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="I23" s="14" t="s">
+      <c r="I23" s="12" t="s">
         <v>107</v>
       </c>
-      <c r="J23" s="15">
+      <c r="J23" s="13">
         <v>0.34</v>
       </c>
-      <c r="K23" s="5" t="s">
-        <v>406</v>
-      </c>
-      <c r="L23" s="7"/>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K23" s="20" t="s">
+        <v>412</v>
+      </c>
+      <c r="L23" s="5"/>
+      <c r="M23" s="5"/>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>10</v>
       </c>
-      <c r="B24" s="14" t="s">
+      <c r="B24" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="C24" s="12" t="s">
+      <c r="C24" s="10" t="s">
         <v>61</v>
       </c>
       <c r="D24" t="s">
         <v>36</v>
       </c>
-      <c r="E24" s="14" t="s">
+      <c r="E24" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="G24" s="14" t="s">
+      <c r="G24" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="H24" s="14" t="s">
+      <c r="H24" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="I24" s="14" t="s">
+      <c r="I24" s="12" t="s">
         <v>107</v>
       </c>
-      <c r="J24" s="15">
+      <c r="J24" s="13">
         <v>0.34</v>
       </c>
-      <c r="K24" s="5" t="s">
-        <v>406</v>
-      </c>
-      <c r="L24" s="7"/>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K24" s="20" t="s">
+        <v>413</v>
+      </c>
+      <c r="L24" s="5"/>
+      <c r="M24" s="5"/>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>10</v>
       </c>
-      <c r="B25" s="14" t="s">
+      <c r="B25" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="C25" s="12" t="s">
+      <c r="C25" s="10" t="s">
         <v>66</v>
       </c>
       <c r="D25" t="s">
         <v>36</v>
       </c>
-      <c r="E25" s="14" t="s">
+      <c r="E25" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="G25" s="14" t="s">
+      <c r="G25" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="H25" s="14" t="s">
+      <c r="H25" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="I25" s="14" t="s">
+      <c r="I25" s="12" t="s">
         <v>107</v>
       </c>
-      <c r="J25" s="15">
+      <c r="J25" s="13">
         <v>0.34</v>
       </c>
-      <c r="K25" s="5" t="s">
-        <v>406</v>
-      </c>
-      <c r="L25" s="7"/>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K25" s="20" t="s">
+        <v>412</v>
+      </c>
+      <c r="L25" s="5"/>
+      <c r="M25" s="5"/>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>10</v>
       </c>
       <c r="B26" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="C26" s="12" t="s">
+      <c r="C26" s="10" t="s">
         <v>68</v>
       </c>
       <c r="D26" t="s">
         <v>36</v>
       </c>
-      <c r="E26" s="14" t="s">
+      <c r="E26" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="G26" s="14" t="s">
+      <c r="G26" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="H26" s="14" t="s">
+      <c r="H26" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="I26" s="14" t="s">
+      <c r="I26" s="12" t="s">
         <v>107</v>
       </c>
-      <c r="J26" s="15">
+      <c r="J26" s="13">
         <v>0.34</v>
       </c>
-      <c r="K26" s="5" t="s">
-        <v>406</v>
-      </c>
-      <c r="L26" s="7"/>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K26" s="20" t="s">
+        <v>412</v>
+      </c>
+      <c r="L26" s="5"/>
+      <c r="M26" s="5"/>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>69</v>
       </c>
       <c r="B27" s="12" t="s">
         <v>70</v>
       </c>
-      <c r="C27" s="12" t="s">
+      <c r="C27" s="10" t="s">
         <v>71</v>
       </c>
       <c r="D27" t="s">
         <v>36</v>
       </c>
-      <c r="E27" s="14" t="s">
+      <c r="E27" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="G27" s="14" t="s">
+      <c r="G27" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="H27" s="14" t="s">
+      <c r="H27" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="I27" s="14" t="s">
+      <c r="I27" s="12" t="s">
         <v>107</v>
       </c>
-      <c r="J27" s="15">
+      <c r="J27" s="13">
         <v>0.34</v>
       </c>
-      <c r="K27" s="5" t="s">
-        <v>406</v>
-      </c>
-      <c r="L27" s="7"/>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K27" s="20" t="s">
+        <v>412</v>
+      </c>
+      <c r="L27" s="5"/>
+      <c r="M27" s="5"/>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>72</v>
       </c>
-      <c r="B28" s="14" t="s">
+      <c r="B28" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="C28" s="12" t="s">
-        <v>383</v>
+      <c r="C28" s="10" t="s">
+        <v>378</v>
       </c>
       <c r="D28" t="s">
         <v>75</v>
       </c>
-      <c r="E28" s="14" t="s">
+      <c r="E28" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="G28" s="14" t="s">
+      <c r="G28" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="H28" s="14" t="s">
+      <c r="H28" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="I28" s="14" t="s">
+      <c r="I28" s="12" t="s">
         <v>107</v>
       </c>
-      <c r="J28" s="15">
+      <c r="J28" s="13">
         <v>0.34</v>
       </c>
-      <c r="K28" s="5" t="s">
-        <v>406</v>
-      </c>
-      <c r="L28" s="7"/>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K28" s="20" t="s">
+        <v>412</v>
+      </c>
+      <c r="L28" s="5"/>
+      <c r="M28" s="5"/>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>72</v>
       </c>
-      <c r="B29" s="14" t="s">
-        <v>382</v>
-      </c>
-      <c r="C29" s="12" t="s">
+      <c r="B29" s="12" t="s">
+        <v>377</v>
+      </c>
+      <c r="C29" s="10" t="s">
         <v>74</v>
       </c>
       <c r="D29" t="s">
         <v>75</v>
       </c>
-      <c r="E29" s="14" t="s">
+      <c r="E29" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="G29" s="14" t="s">
+      <c r="G29" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="H29" s="14" t="s">
+      <c r="H29" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="I29" s="14" t="s">
+      <c r="I29" s="12" t="s">
         <v>107</v>
       </c>
-      <c r="J29" s="15">
+      <c r="J29" s="13">
         <v>0.34</v>
       </c>
-      <c r="K29" s="5" t="s">
-        <v>406</v>
-      </c>
-      <c r="L29" s="7"/>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K29" s="20" t="s">
+        <v>412</v>
+      </c>
+      <c r="L29" s="5"/>
+      <c r="M29" s="5"/>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>76</v>
       </c>
-      <c r="B30" s="14" t="s">
+      <c r="B30" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="C30" s="12" t="s">
+      <c r="C30" s="10" t="s">
         <v>78</v>
       </c>
       <c r="D30" t="s">
         <v>36</v>
       </c>
-      <c r="E30" s="14" t="s">
+      <c r="E30" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="G30" s="14" t="s">
+      <c r="G30" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="H30" s="14" t="s">
+      <c r="H30" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="I30" s="14" t="s">
+      <c r="I30" s="12" t="s">
         <v>107</v>
       </c>
-      <c r="J30" s="15">
+      <c r="J30" s="13">
         <v>0.34</v>
       </c>
-      <c r="K30" s="5" t="s">
-        <v>406</v>
-      </c>
-      <c r="L30" s="7"/>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K30" s="20" t="s">
+        <v>412</v>
+      </c>
+      <c r="L30" s="5"/>
+      <c r="M30" s="5"/>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>58</v>
       </c>
       <c r="B31" s="12" t="s">
         <v>79</v>
       </c>
-      <c r="C31" s="12" t="s">
-        <v>410</v>
+      <c r="C31" s="10" t="s">
+        <v>404</v>
       </c>
       <c r="D31" t="s">
         <v>36</v>
       </c>
-      <c r="E31" s="14" t="s">
+      <c r="E31" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="G31" s="14" t="s">
+      <c r="G31" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="H31" s="14" t="s">
+      <c r="H31" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="I31" s="14" t="s">
+      <c r="I31" s="12" t="s">
         <v>107</v>
       </c>
-      <c r="J31" s="15">
+      <c r="J31" s="13">
         <v>0.34</v>
       </c>
-      <c r="K31" s="5" t="s">
-        <v>406</v>
-      </c>
-      <c r="L31" s="7"/>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K31" s="20" t="s">
+        <v>412</v>
+      </c>
+      <c r="L31" s="5"/>
+      <c r="M31" s="5"/>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>97</v>
       </c>
-      <c r="B32" s="14" t="s">
+      <c r="B32" s="12" t="s">
         <v>98</v>
       </c>
-      <c r="C32" s="12" t="s">
+      <c r="C32" s="10" t="s">
         <v>99</v>
       </c>
       <c r="D32" t="s">
         <v>36</v>
       </c>
-      <c r="E32" s="14" t="s">
+      <c r="E32" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="G32" s="14" t="s">
+      <c r="G32" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="H32" s="14" t="s">
+      <c r="H32" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="I32" s="14" t="s">
+      <c r="I32" s="12" t="s">
         <v>107</v>
       </c>
-      <c r="J32" s="15">
+      <c r="J32" s="13">
         <v>0.34</v>
       </c>
-      <c r="K32" s="5" t="s">
-        <v>406</v>
-      </c>
-      <c r="L32" s="7"/>
-    </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K32" s="20" t="s">
+        <v>412</v>
+      </c>
+      <c r="L32" s="5"/>
+      <c r="M32" s="5"/>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>381</v>
-      </c>
-      <c r="B33" s="14" t="s">
+        <v>376</v>
+      </c>
+      <c r="B33" s="12" t="s">
         <v>80</v>
       </c>
-      <c r="C33" s="12" t="s">
+      <c r="C33" s="10" t="s">
         <v>81</v>
       </c>
       <c r="D33" t="s">
         <v>82</v>
       </c>
-      <c r="E33" s="14" t="s">
+      <c r="E33" s="12" t="s">
         <v>83</v>
       </c>
-      <c r="G33" s="14" t="s">
+      <c r="G33" s="12" t="s">
         <v>84</v>
       </c>
-      <c r="H33" s="14" t="s">
+      <c r="H33" s="12" t="s">
         <v>85</v>
       </c>
-      <c r="I33" s="14" t="s">
+      <c r="I33" s="12" t="s">
         <v>108</v>
       </c>
-      <c r="J33" s="15">
+      <c r="J33" s="13">
         <v>0.4</v>
       </c>
-      <c r="K33" s="5" t="s">
+      <c r="K33" s="20" t="s">
         <v>86</v>
       </c>
-      <c r="L33" s="7"/>
-    </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="L33" s="5"/>
+      <c r="M33" s="5"/>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>16</v>
       </c>
-      <c r="B34" s="14" t="s">
+      <c r="B34" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="C34" s="12" t="s">
+      <c r="C34" s="10" t="s">
         <v>88</v>
       </c>
       <c r="D34" t="s">
         <v>82</v>
       </c>
-      <c r="E34" s="14" t="s">
+      <c r="E34" s="12" t="s">
         <v>83</v>
       </c>
-      <c r="G34" s="14" t="s">
+      <c r="G34" s="12" t="s">
         <v>84</v>
       </c>
-      <c r="H34" s="14" t="s">
+      <c r="H34" s="12" t="s">
         <v>85</v>
       </c>
-      <c r="I34" s="14" t="s">
+      <c r="I34" s="12" t="s">
         <v>108</v>
       </c>
-      <c r="J34" s="15">
+      <c r="J34" s="13">
         <v>0.4</v>
       </c>
-      <c r="K34" s="5" t="s">
+      <c r="K34" s="20" t="s">
         <v>86</v>
       </c>
-      <c r="L34" s="7"/>
-    </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="L34" s="5"/>
+      <c r="M34" s="5"/>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>16</v>
       </c>
       <c r="B35" s="12" t="s">
         <v>89</v>
       </c>
-      <c r="C35" s="12" t="s">
+      <c r="C35" s="10" t="s">
         <v>88</v>
       </c>
       <c r="D35" t="s">
         <v>82</v>
       </c>
-      <c r="E35" s="14" t="s">
+      <c r="E35" s="12" t="s">
         <v>83</v>
       </c>
-      <c r="G35" s="14" t="s">
+      <c r="G35" s="12" t="s">
         <v>84</v>
       </c>
-      <c r="H35" s="14" t="s">
+      <c r="H35" s="12" t="s">
         <v>85</v>
       </c>
-      <c r="I35" s="14" t="s">
+      <c r="I35" s="12" t="s">
         <v>108</v>
       </c>
-      <c r="J35" s="15">
+      <c r="J35" s="13">
         <v>0.4</v>
       </c>
-      <c r="K35" s="5" t="s">
+      <c r="K35" s="20" t="s">
         <v>86</v>
       </c>
-      <c r="L35" s="7"/>
-    </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="L35" s="5"/>
+      <c r="M35" s="5"/>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>90</v>
       </c>
-      <c r="B36" s="14" t="s">
+      <c r="B36" s="12" t="s">
         <v>91</v>
       </c>
-      <c r="C36" s="12" t="s">
+      <c r="C36" s="10" t="s">
         <v>92</v>
       </c>
       <c r="D36" t="s">
         <v>82</v>
       </c>
-      <c r="E36" s="14" t="s">
+      <c r="E36" s="12" t="s">
         <v>83</v>
       </c>
-      <c r="G36" s="14" t="s">
+      <c r="G36" s="12" t="s">
         <v>84</v>
       </c>
-      <c r="H36" s="14" t="s">
+      <c r="H36" s="12" t="s">
         <v>85</v>
       </c>
-      <c r="I36" s="14" t="s">
+      <c r="I36" s="12" t="s">
         <v>108</v>
       </c>
-      <c r="J36" s="15">
+      <c r="J36" s="13">
         <v>0.4</v>
       </c>
-      <c r="K36" s="5" t="s">
+      <c r="K36" s="20" t="s">
         <v>86</v>
       </c>
-      <c r="L36" s="7"/>
-    </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="L36" s="5"/>
+      <c r="M36" s="5"/>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>93</v>
       </c>
-      <c r="B37" s="14" t="s">
+      <c r="B37" s="12" t="s">
         <v>94</v>
       </c>
-      <c r="C37" s="12" t="s">
+      <c r="C37" s="10" t="s">
         <v>92</v>
       </c>
       <c r="D37" t="s">
         <v>82</v>
       </c>
-      <c r="E37" s="14" t="s">
+      <c r="E37" s="12" t="s">
         <v>83</v>
       </c>
-      <c r="G37" s="14" t="s">
+      <c r="G37" s="12" t="s">
         <v>84</v>
       </c>
-      <c r="H37" s="14" t="s">
+      <c r="H37" s="12" t="s">
         <v>85</v>
       </c>
-      <c r="I37" s="14" t="s">
+      <c r="I37" s="12" t="s">
         <v>108</v>
       </c>
-      <c r="J37" s="15">
+      <c r="J37" s="13">
         <v>0.4</v>
       </c>
-      <c r="K37" s="5" t="s">
+      <c r="K37" s="20" t="s">
         <v>86</v>
       </c>
-      <c r="L37" s="7"/>
-    </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="L37" s="5"/>
+      <c r="M37" s="5"/>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>93</v>
       </c>
-      <c r="B38" s="14" t="s">
+      <c r="B38" s="12" t="s">
         <v>95</v>
       </c>
-      <c r="C38" s="12" t="s">
+      <c r="C38" s="10" t="s">
         <v>92</v>
       </c>
       <c r="D38" t="s">
         <v>96</v>
       </c>
-      <c r="E38" s="14" t="s">
+      <c r="E38" s="12" t="s">
         <v>83</v>
       </c>
-      <c r="G38" s="14" t="s">
+      <c r="G38" s="12" t="s">
         <v>84</v>
       </c>
-      <c r="H38" s="14" t="s">
+      <c r="H38" s="12" t="s">
         <v>85</v>
       </c>
-      <c r="I38" s="14" t="s">
+      <c r="I38" s="12" t="s">
         <v>108</v>
       </c>
-      <c r="J38" s="15">
+      <c r="J38" s="13">
         <v>0.4</v>
       </c>
-      <c r="K38" s="5" t="s">
+      <c r="K38" s="20" t="s">
         <v>86</v>
       </c>
-      <c r="L38" s="7"/>
-    </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="L38" s="5"/>
+      <c r="M38" s="5"/>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>103</v>
       </c>
       <c r="B39" s="12" t="s">
         <v>104</v>
       </c>
-      <c r="C39" s="12" t="s">
+      <c r="C39" s="10" t="s">
         <v>105</v>
       </c>
       <c r="D39" t="s">
         <v>106</v>
       </c>
-      <c r="E39" s="14" t="s">
+      <c r="E39" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="G39" s="14" t="s">
+      <c r="G39" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="H39" s="14" t="s">
+      <c r="H39" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="I39" s="14" t="s">
+      <c r="I39" s="12" t="s">
         <v>107</v>
       </c>
-      <c r="J39" s="15">
+      <c r="J39" s="13">
         <v>0.34</v>
       </c>
-      <c r="K39" s="5" t="s">
-        <v>406</v>
-      </c>
-      <c r="L39" s="7"/>
-    </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="F40" s="2"/>
-      <c r="G40" s="2"/>
-      <c r="H40" s="2"/>
-      <c r="I40" s="2"/>
-      <c r="J40" s="4"/>
-      <c r="K40" s="5"/>
-      <c r="L40" s="3"/>
+      <c r="K39" s="20" t="s">
+        <v>412</v>
+      </c>
+      <c r="L39" s="5"/>
+      <c r="M39" s="5"/>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B40" s="12"/>
+      <c r="C40" s="10"/>
+      <c r="E40" s="12"/>
+      <c r="G40" s="12"/>
+      <c r="H40" s="12"/>
+      <c r="I40" s="12"/>
+      <c r="J40" s="13"/>
+      <c r="K40" s="20"/>
+      <c r="L40" s="5"/>
+      <c r="M40" s="5"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K39">
@@ -3204,15 +3300,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87C01629-0328-48DC-A4F4-B3C50775B1B9}">
-  <dimension ref="A1:D117"/>
+  <dimension ref="A1:D130"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="A126" sqref="A126"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.33203125" customWidth="1"/>
+    <col min="1" max="1" width="28.109375" customWidth="1"/>
     <col min="2" max="2" width="21.109375" customWidth="1"/>
     <col min="3" max="3" width="49.33203125" customWidth="1"/>
     <col min="4" max="4" width="20.109375" customWidth="1"/>
@@ -3240,7 +3336,7 @@
         <v>117</v>
       </c>
       <c r="C2" t="s">
-        <v>384</v>
+        <v>379</v>
       </c>
       <c r="D2" t="s">
         <v>118</v>
@@ -3254,7 +3350,7 @@
         <v>117</v>
       </c>
       <c r="C3" t="s">
-        <v>385</v>
+        <v>380</v>
       </c>
       <c r="D3" t="s">
         <v>120</v>
@@ -3268,7 +3364,7 @@
         <v>117</v>
       </c>
       <c r="C4" t="s">
-        <v>386</v>
+        <v>381</v>
       </c>
       <c r="D4" t="s">
         <v>120</v>
@@ -3282,7 +3378,7 @@
         <v>117</v>
       </c>
       <c r="C5" t="s">
-        <v>387</v>
+        <v>382</v>
       </c>
       <c r="D5" t="s">
         <v>121</v>
@@ -3296,7 +3392,7 @@
         <v>122</v>
       </c>
       <c r="C6" t="s">
-        <v>388</v>
+        <v>383</v>
       </c>
       <c r="D6" t="s">
         <v>123</v>
@@ -3310,7 +3406,7 @@
         <v>122</v>
       </c>
       <c r="C7" t="s">
-        <v>389</v>
+        <v>384</v>
       </c>
       <c r="D7" t="s">
         <v>123</v>
@@ -3324,7 +3420,7 @@
         <v>122</v>
       </c>
       <c r="C8" t="s">
-        <v>385</v>
+        <v>380</v>
       </c>
       <c r="D8" t="s">
         <v>125</v>
@@ -3338,7 +3434,7 @@
         <v>122</v>
       </c>
       <c r="C9" t="s">
-        <v>390</v>
+        <v>385</v>
       </c>
       <c r="D9" t="s">
         <v>125</v>
@@ -3352,7 +3448,7 @@
         <v>127</v>
       </c>
       <c r="C10" t="s">
-        <v>414</v>
+        <v>408</v>
       </c>
       <c r="D10" t="s">
         <v>128</v>
@@ -3366,7 +3462,7 @@
         <v>127</v>
       </c>
       <c r="C11" t="s">
-        <v>415</v>
+        <v>409</v>
       </c>
       <c r="D11" t="s">
         <v>128</v>
@@ -3380,7 +3476,7 @@
         <v>127</v>
       </c>
       <c r="C12" t="s">
-        <v>416</v>
+        <v>410</v>
       </c>
       <c r="D12" t="s">
         <v>129</v>
@@ -3394,7 +3490,7 @@
         <v>130</v>
       </c>
       <c r="C13" t="s">
-        <v>411</v>
+        <v>405</v>
       </c>
       <c r="D13" t="s">
         <v>131</v>
@@ -3408,7 +3504,7 @@
         <v>130</v>
       </c>
       <c r="C14" t="s">
-        <v>412</v>
+        <v>406</v>
       </c>
       <c r="D14" t="s">
         <v>132</v>
@@ -3608,7 +3704,7 @@
       <c r="C29" t="s">
         <v>155</v>
       </c>
-      <c r="D29" s="8">
+      <c r="D29" s="6">
         <v>52</v>
       </c>
     </row>
@@ -3721,59 +3817,59 @@
         <v>132</v>
       </c>
     </row>
-    <row r="38" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="19" t="s">
+    <row r="38" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="17" t="s">
         <v>165</v>
       </c>
-      <c r="B38" s="19" t="s">
+      <c r="B38" s="17" t="s">
         <v>210</v>
       </c>
-      <c r="C38" s="19" t="s">
+      <c r="C38" s="17" t="s">
         <v>151</v>
       </c>
-      <c r="D38" s="19" t="s">
+      <c r="D38" s="17" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="39" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="19" t="s">
+    <row r="39" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="17" t="s">
         <v>165</v>
       </c>
-      <c r="B39" s="19" t="s">
+      <c r="B39" s="17" t="s">
         <v>210</v>
       </c>
-      <c r="C39" s="19" t="s">
+      <c r="C39" s="17" t="s">
         <v>167</v>
       </c>
-      <c r="D39" s="19" t="s">
+      <c r="D39" s="17" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="40" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="19" t="s">
+    <row r="40" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="17" t="s">
         <v>165</v>
       </c>
-      <c r="B40" s="19" t="s">
+      <c r="B40" s="17" t="s">
         <v>210</v>
       </c>
-      <c r="C40" s="19" t="s">
+      <c r="C40" s="17" t="s">
         <v>168</v>
       </c>
-      <c r="D40" s="19" t="s">
+      <c r="D40" s="17" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="41" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="19" t="s">
+    <row r="41" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="17" t="s">
         <v>165</v>
       </c>
-      <c r="B41" s="19" t="s">
+      <c r="B41" s="17" t="s">
         <v>210</v>
       </c>
-      <c r="C41" s="19" t="s">
+      <c r="C41" s="17" t="s">
         <v>169</v>
       </c>
-      <c r="D41" s="19" t="s">
+      <c r="D41" s="17" t="s">
         <v>129</v>
       </c>
     </row>
@@ -3823,7 +3919,7 @@
       <c r="A45" t="s">
         <v>170</v>
       </c>
-      <c r="B45" s="8">
+      <c r="B45" s="6">
         <v>877</v>
       </c>
       <c r="C45" t="s">
@@ -3837,7 +3933,7 @@
       <c r="A46" t="s">
         <v>170</v>
       </c>
-      <c r="B46" s="8">
+      <c r="B46" s="6">
         <v>877</v>
       </c>
       <c r="C46" t="s">
@@ -3851,7 +3947,7 @@
       <c r="A47" t="s">
         <v>170</v>
       </c>
-      <c r="B47" s="8">
+      <c r="B47" s="6">
         <v>879</v>
       </c>
       <c r="C47" t="s">
@@ -3865,7 +3961,7 @@
       <c r="A48" t="s">
         <v>170</v>
       </c>
-      <c r="B48" s="8">
+      <c r="B48" s="6">
         <v>879</v>
       </c>
       <c r="C48" t="s">
@@ -4065,9 +4161,9 @@
         <v>193</v>
       </c>
       <c r="C62" t="s">
-        <v>391</v>
-      </c>
-      <c r="D62" s="8">
+        <v>386</v>
+      </c>
+      <c r="D62" s="6">
         <v>52</v>
       </c>
     </row>
@@ -4079,9 +4175,9 @@
         <v>193</v>
       </c>
       <c r="C63" t="s">
-        <v>392</v>
-      </c>
-      <c r="D63" s="8">
+        <v>387</v>
+      </c>
+      <c r="D63" s="6">
         <v>52</v>
       </c>
     </row>
@@ -4093,9 +4189,9 @@
         <v>193</v>
       </c>
       <c r="C64" t="s">
-        <v>393</v>
-      </c>
-      <c r="D64" s="8">
+        <v>388</v>
+      </c>
+      <c r="D64" s="6">
         <v>52</v>
       </c>
     </row>
@@ -4107,9 +4203,9 @@
         <v>193</v>
       </c>
       <c r="C65" t="s">
-        <v>394</v>
-      </c>
-      <c r="D65" s="8">
+        <v>389</v>
+      </c>
+      <c r="D65" s="6">
         <v>52</v>
       </c>
     </row>
@@ -4121,9 +4217,9 @@
         <v>193</v>
       </c>
       <c r="C66" t="s">
-        <v>395</v>
-      </c>
-      <c r="D66" s="8">
+        <v>390</v>
+      </c>
+      <c r="D66" s="6">
         <v>52</v>
       </c>
     </row>
@@ -4135,9 +4231,9 @@
         <v>193</v>
       </c>
       <c r="C67" t="s">
-        <v>396</v>
-      </c>
-      <c r="D67" s="8">
+        <v>391</v>
+      </c>
+      <c r="D67" s="6">
         <v>50</v>
       </c>
     </row>
@@ -4149,9 +4245,9 @@
         <v>193</v>
       </c>
       <c r="C68" t="s">
-        <v>397</v>
-      </c>
-      <c r="D68" s="8">
+        <v>392</v>
+      </c>
+      <c r="D68" s="6">
         <v>50</v>
       </c>
     </row>
@@ -4163,9 +4259,9 @@
         <v>193</v>
       </c>
       <c r="C69" t="s">
-        <v>398</v>
-      </c>
-      <c r="D69" s="8">
+        <v>393</v>
+      </c>
+      <c r="D69" s="6">
         <v>50</v>
       </c>
     </row>
@@ -4177,9 +4273,9 @@
         <v>193</v>
       </c>
       <c r="C70" t="s">
-        <v>399</v>
-      </c>
-      <c r="D70" s="8">
+        <v>394</v>
+      </c>
+      <c r="D70" s="6">
         <v>50</v>
       </c>
     </row>
@@ -4191,9 +4287,9 @@
         <v>193</v>
       </c>
       <c r="C71" t="s">
-        <v>400</v>
-      </c>
-      <c r="D71" s="8">
+        <v>395</v>
+      </c>
+      <c r="D71" s="6">
         <v>48</v>
       </c>
     </row>
@@ -4205,9 +4301,9 @@
         <v>193</v>
       </c>
       <c r="C72" t="s">
-        <v>401</v>
-      </c>
-      <c r="D72" s="8">
+        <v>396</v>
+      </c>
+      <c r="D72" s="6">
         <v>48</v>
       </c>
     </row>
@@ -4219,9 +4315,9 @@
         <v>193</v>
       </c>
       <c r="C73" t="s">
-        <v>402</v>
-      </c>
-      <c r="D73" s="8">
+        <v>397</v>
+      </c>
+      <c r="D73" s="6">
         <v>48</v>
       </c>
     </row>
@@ -4233,9 +4329,9 @@
         <v>193</v>
       </c>
       <c r="C74" t="s">
-        <v>403</v>
-      </c>
-      <c r="D74" s="8">
+        <v>398</v>
+      </c>
+      <c r="D74" s="6">
         <v>48</v>
       </c>
     </row>
@@ -4247,9 +4343,9 @@
         <v>193</v>
       </c>
       <c r="C75" t="s">
-        <v>404</v>
-      </c>
-      <c r="D75" s="8" t="s">
+        <v>399</v>
+      </c>
+      <c r="D75" s="6" t="s">
         <v>118</v>
       </c>
     </row>
@@ -4261,9 +4357,9 @@
         <v>193</v>
       </c>
       <c r="C76" t="s">
-        <v>405</v>
-      </c>
-      <c r="D76" s="8" t="s">
+        <v>400</v>
+      </c>
+      <c r="D76" s="6" t="s">
         <v>129</v>
       </c>
     </row>
@@ -4277,7 +4373,7 @@
       <c r="C77" t="s">
         <v>195</v>
       </c>
-      <c r="D77" s="8" t="s">
+      <c r="D77" s="6" t="s">
         <v>132</v>
       </c>
     </row>
@@ -4291,7 +4387,7 @@
       <c r="C78" t="s">
         <v>147</v>
       </c>
-      <c r="D78" s="8" t="s">
+      <c r="D78" s="6" t="s">
         <v>150</v>
       </c>
     </row>
@@ -4305,7 +4401,7 @@
       <c r="C79" t="s">
         <v>147</v>
       </c>
-      <c r="D79" s="8">
+      <c r="D79" s="6">
         <v>48</v>
       </c>
     </row>
@@ -4319,7 +4415,7 @@
       <c r="C80" t="s">
         <v>147</v>
       </c>
-      <c r="D80" s="8" t="s">
+      <c r="D80" s="6" t="s">
         <v>120</v>
       </c>
     </row>
@@ -4333,7 +4429,7 @@
       <c r="C81" t="s">
         <v>147</v>
       </c>
-      <c r="D81" s="8" t="s">
+      <c r="D81" s="6" t="s">
         <v>128</v>
       </c>
     </row>
@@ -4347,7 +4443,7 @@
       <c r="C82" t="s">
         <v>147</v>
       </c>
-      <c r="D82" s="8">
+      <c r="D82" s="6">
         <v>52</v>
       </c>
     </row>
@@ -4482,10 +4578,10 @@
         <v>208</v>
       </c>
       <c r="B92" t="s">
-        <v>372</v>
+        <v>367</v>
       </c>
       <c r="C92" t="s">
-        <v>373</v>
+        <v>368</v>
       </c>
       <c r="D92" t="s">
         <v>132</v>
@@ -4496,13 +4592,13 @@
         <v>208</v>
       </c>
       <c r="B93" t="s">
-        <v>374</v>
+        <v>369</v>
       </c>
       <c r="C93" t="s">
-        <v>373</v>
+        <v>368</v>
       </c>
       <c r="D93" t="s">
-        <v>375</v>
+        <v>370</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.3">
@@ -4510,10 +4606,10 @@
         <v>208</v>
       </c>
       <c r="B94" t="s">
-        <v>376</v>
+        <v>371</v>
       </c>
       <c r="C94" t="s">
-        <v>373</v>
+        <v>368</v>
       </c>
       <c r="D94" t="s">
         <v>132</v>
@@ -4524,10 +4620,10 @@
         <v>208</v>
       </c>
       <c r="B95" t="s">
-        <v>377</v>
+        <v>372</v>
       </c>
       <c r="C95" t="s">
-        <v>373</v>
+        <v>368</v>
       </c>
       <c r="D95" t="s">
         <v>132</v>
@@ -4538,7 +4634,7 @@
         <v>208</v>
       </c>
       <c r="B96" t="s">
-        <v>372</v>
+        <v>367</v>
       </c>
       <c r="C96" t="s">
         <v>159</v>
@@ -4552,7 +4648,7 @@
         <v>208</v>
       </c>
       <c r="B97" t="s">
-        <v>374</v>
+        <v>369</v>
       </c>
       <c r="C97" t="s">
         <v>159</v>
@@ -4566,7 +4662,7 @@
         <v>208</v>
       </c>
       <c r="B98" t="s">
-        <v>376</v>
+        <v>371</v>
       </c>
       <c r="C98" t="s">
         <v>159</v>
@@ -4580,7 +4676,7 @@
         <v>208</v>
       </c>
       <c r="B99" t="s">
-        <v>377</v>
+        <v>372</v>
       </c>
       <c r="C99" t="s">
         <v>159</v>
@@ -4839,6 +4935,188 @@
       </c>
       <c r="D117" t="s">
         <v>131</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A118" t="s">
+        <v>414</v>
+      </c>
+      <c r="B118" t="s">
+        <v>419</v>
+      </c>
+      <c r="C118" t="s">
+        <v>147</v>
+      </c>
+      <c r="D118" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A119" t="s">
+        <v>414</v>
+      </c>
+      <c r="B119" t="s">
+        <v>421</v>
+      </c>
+      <c r="C119" t="s">
+        <v>147</v>
+      </c>
+      <c r="D119" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A120" t="s">
+        <v>414</v>
+      </c>
+      <c r="B120" t="s">
+        <v>420</v>
+      </c>
+      <c r="C120" t="s">
+        <v>147</v>
+      </c>
+      <c r="D120" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A121" t="s">
+        <v>425</v>
+      </c>
+      <c r="B121" s="18" t="s">
+        <v>142</v>
+      </c>
+      <c r="C121" t="s">
+        <v>159</v>
+      </c>
+      <c r="D121" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A122" t="s">
+        <v>425</v>
+      </c>
+      <c r="B122" s="18" t="s">
+        <v>142</v>
+      </c>
+      <c r="C122" t="s">
+        <v>368</v>
+      </c>
+      <c r="D122" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A123" t="s">
+        <v>425</v>
+      </c>
+      <c r="B123" t="s">
+        <v>422</v>
+      </c>
+      <c r="C123" t="s">
+        <v>159</v>
+      </c>
+      <c r="D123" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A124" t="s">
+        <v>425</v>
+      </c>
+      <c r="B124" s="18" t="s">
+        <v>422</v>
+      </c>
+      <c r="C124" t="s">
+        <v>368</v>
+      </c>
+      <c r="D124" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A125" t="s">
+        <v>425</v>
+      </c>
+      <c r="B125" t="s">
+        <v>423</v>
+      </c>
+      <c r="C125" t="s">
+        <v>368</v>
+      </c>
+      <c r="D125" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A126" t="s">
+        <v>425</v>
+      </c>
+      <c r="B126" t="s">
+        <v>423</v>
+      </c>
+      <c r="C126" t="s">
+        <v>159</v>
+      </c>
+      <c r="D126" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A127" t="s">
+        <v>425</v>
+      </c>
+      <c r="B127" t="s">
+        <v>424</v>
+      </c>
+      <c r="C127" t="s">
+        <v>368</v>
+      </c>
+      <c r="D127" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A128" t="s">
+        <v>425</v>
+      </c>
+      <c r="B128" t="s">
+        <v>424</v>
+      </c>
+      <c r="C128" t="s">
+        <v>159</v>
+      </c>
+      <c r="D128" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A129" t="s">
+        <v>425</v>
+      </c>
+      <c r="B129" t="s">
+        <v>146</v>
+      </c>
+      <c r="C129" t="s">
+        <v>368</v>
+      </c>
+      <c r="D129" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A130" t="s">
+        <v>425</v>
+      </c>
+      <c r="B130" t="s">
+        <v>146</v>
+      </c>
+      <c r="C130" t="s">
+        <v>159</v>
+      </c>
+      <c r="D130" t="s">
+        <v>223</v>
       </c>
     </row>
   </sheetData>
@@ -4848,17 +5126,21 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43C2BCAE-C18D-46A7-93FE-4E59012F3E5E}">
-  <dimension ref="A1:K25"/>
+  <dimension ref="A1:K26"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="24.6640625" customWidth="1"/>
-    <col min="3" max="3" width="36.109375" customWidth="1"/>
+    <col min="1" max="1" width="15" customWidth="1"/>
+    <col min="2" max="2" width="10.109375" customWidth="1"/>
+    <col min="3" max="3" width="50.88671875" customWidth="1"/>
     <col min="4" max="4" width="105.88671875" customWidth="1"/>
+    <col min="5" max="5" width="12.109375" customWidth="1"/>
+    <col min="6" max="6" width="12" customWidth="1"/>
+    <col min="7" max="7" width="18.77734375" customWidth="1"/>
     <col min="8" max="8" width="61.5546875" customWidth="1"/>
     <col min="9" max="9" width="57.109375" customWidth="1"/>
     <col min="10" max="10" width="35.5546875" customWidth="1"/>
@@ -4927,7 +5209,7 @@
       <c r="J2" t="s">
         <v>250</v>
       </c>
-      <c r="K2" s="9">
+      <c r="K2" s="7">
         <v>395</v>
       </c>
     </row>
@@ -4959,7 +5241,7 @@
       <c r="J3" t="s">
         <v>258</v>
       </c>
-      <c r="K3" s="9">
+      <c r="K3" s="7">
         <v>195</v>
       </c>
     </row>
@@ -4982,10 +5264,10 @@
       <c r="G4" t="s">
         <v>247</v>
       </c>
-      <c r="H4" s="10" t="s">
+      <c r="H4" s="8" t="s">
         <v>262</v>
       </c>
-      <c r="I4" s="18" t="s">
+      <c r="I4" s="16" t="s">
         <v>249</v>
       </c>
       <c r="J4" t="s">
@@ -5020,7 +5302,7 @@
       <c r="J5" t="s">
         <v>269</v>
       </c>
-      <c r="K5" s="9">
+      <c r="K5" s="7">
         <v>295</v>
       </c>
     </row>
@@ -5052,7 +5334,7 @@
       <c r="J6" t="s">
         <v>275</v>
       </c>
-      <c r="K6" s="9">
+      <c r="K6" s="7">
         <v>395</v>
       </c>
     </row>
@@ -5084,19 +5366,19 @@
       <c r="J7" t="s">
         <v>280</v>
       </c>
-      <c r="K7" s="9">
+      <c r="K7" s="7">
         <v>295</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>281</v>
       </c>
       <c r="C8" t="s">
         <v>282</v>
       </c>
-      <c r="D8" t="s">
-        <v>283</v>
+      <c r="D8" s="3" t="s">
+        <v>426</v>
       </c>
       <c r="E8">
         <v>0.39</v>
@@ -5108,27 +5390,27 @@
         <v>255</v>
       </c>
       <c r="H8" t="s">
+        <v>283</v>
+      </c>
+      <c r="I8" t="s">
         <v>284</v>
       </c>
-      <c r="I8" t="s">
+      <c r="J8" t="s">
         <v>285</v>
       </c>
-      <c r="J8" t="s">
-        <v>286</v>
-      </c>
-      <c r="K8" s="9">
+      <c r="K8" s="7">
         <v>189</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
+        <v>286</v>
+      </c>
+      <c r="C9" t="s">
         <v>287</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>288</v>
-      </c>
-      <c r="D9" t="s">
-        <v>289</v>
       </c>
       <c r="E9">
         <v>0.09</v>
@@ -5140,27 +5422,27 @@
         <v>255</v>
       </c>
       <c r="H9" t="s">
+        <v>289</v>
+      </c>
+      <c r="I9" s="2" t="s">
         <v>290</v>
       </c>
-      <c r="I9" s="2" t="s">
+      <c r="J9" t="s">
         <v>291</v>
       </c>
-      <c r="J9" t="s">
-        <v>292</v>
-      </c>
-      <c r="K9" s="11">
+      <c r="K9" s="9">
         <v>59</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
+        <v>292</v>
+      </c>
+      <c r="C10" t="s">
         <v>293</v>
       </c>
-      <c r="C10" t="s">
-        <v>294</v>
-      </c>
       <c r="D10" t="s">
-        <v>295</v>
+        <v>427</v>
       </c>
       <c r="E10">
         <v>0.9</v>
@@ -5172,27 +5454,27 @@
         <v>255</v>
       </c>
       <c r="H10" t="s">
+        <v>294</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>295</v>
+      </c>
+      <c r="J10" t="s">
         <v>296</v>
       </c>
-      <c r="I10" t="s">
+      <c r="K10" s="9">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="B11" t="s">
         <v>297</v>
       </c>
-      <c r="J10" t="s">
+      <c r="C11" t="s">
         <v>298</v>
       </c>
-      <c r="K10" s="11">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B11" t="s">
-        <v>299</v>
-      </c>
-      <c r="C11" t="s">
-        <v>300</v>
-      </c>
-      <c r="D11" t="s">
-        <v>301</v>
+      <c r="D11" s="3" t="s">
+        <v>429</v>
       </c>
       <c r="E11">
         <v>0.25</v>
@@ -5203,25 +5485,25 @@
       <c r="G11" t="s">
         <v>255</v>
       </c>
-      <c r="H11" s="18" t="s">
-        <v>409</v>
-      </c>
-      <c r="I11" s="18" t="s">
-        <v>302</v>
+      <c r="H11" s="16" t="s">
+        <v>403</v>
+      </c>
+      <c r="I11" s="16" t="s">
+        <v>299</v>
       </c>
       <c r="J11" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="C12" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="D12" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="E12">
         <v>0.9</v>
@@ -5233,27 +5515,27 @@
         <v>255</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="I12" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="J12" t="s">
-        <v>307</v>
-      </c>
-      <c r="K12" s="9">
+        <v>304</v>
+      </c>
+      <c r="K12" s="7">
         <v>129</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="C13" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="D13" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="E13">
         <v>0.15</v>
@@ -5265,27 +5547,27 @@
         <v>255</v>
       </c>
       <c r="H13" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="I13" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="J13" t="s">
-        <v>313</v>
-      </c>
-      <c r="K13" s="9">
+        <v>310</v>
+      </c>
+      <c r="K13" s="7">
         <v>265</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="C14" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="D14" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="E14">
         <v>0.09</v>
@@ -5296,25 +5578,25 @@
       <c r="G14" t="s">
         <v>255</v>
       </c>
-      <c r="H14" s="18" t="s">
-        <v>408</v>
-      </c>
-      <c r="I14" s="10" t="s">
-        <v>317</v>
+      <c r="H14" s="16" t="s">
+        <v>402</v>
+      </c>
+      <c r="I14" s="8" t="s">
+        <v>314</v>
       </c>
       <c r="J14" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="C15" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="D15" t="s">
-        <v>321</v>
+        <v>428</v>
       </c>
       <c r="E15">
         <v>0.13</v>
@@ -5325,28 +5607,28 @@
       <c r="G15" t="s">
         <v>255</v>
       </c>
-      <c r="H15" t="s">
-        <v>322</v>
-      </c>
-      <c r="I15" t="s">
-        <v>323</v>
+      <c r="H15" s="16" t="s">
+        <v>318</v>
+      </c>
+      <c r="I15" s="8" t="s">
+        <v>319</v>
       </c>
       <c r="J15" t="s">
-        <v>324</v>
-      </c>
-      <c r="K15" s="9">
+        <v>320</v>
+      </c>
+      <c r="K15">
         <v>195</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="C16" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
       <c r="D16" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
       <c r="E16">
         <v>0.32</v>
@@ -5358,27 +5640,27 @@
         <v>255</v>
       </c>
       <c r="H16" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
       <c r="I16" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="J16" t="s">
-        <v>329</v>
-      </c>
-      <c r="K16" s="9">
+        <v>325</v>
+      </c>
+      <c r="K16" s="7">
         <v>195</v>
       </c>
     </row>
     <row r="17" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
       <c r="C17" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="D17" t="s">
-        <v>331</v>
+        <v>418</v>
       </c>
       <c r="E17">
         <v>0.5</v>
@@ -5390,27 +5672,27 @@
         <v>255</v>
       </c>
       <c r="H17" t="s">
-        <v>332</v>
+        <v>327</v>
       </c>
       <c r="I17" t="s">
-        <v>333</v>
+        <v>328</v>
       </c>
       <c r="J17" t="s">
-        <v>334</v>
-      </c>
-      <c r="K17" s="9">
+        <v>329</v>
+      </c>
+      <c r="K17" s="7">
         <v>195</v>
       </c>
     </row>
     <row r="18" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
       <c r="C18" t="s">
-        <v>336</v>
+        <v>331</v>
       </c>
       <c r="D18" t="s">
-        <v>337</v>
+        <v>332</v>
       </c>
       <c r="E18">
         <v>0.09</v>
@@ -5422,27 +5704,27 @@
         <v>255</v>
       </c>
       <c r="H18" t="s">
-        <v>338</v>
+        <v>333</v>
       </c>
       <c r="I18" t="s">
-        <v>339</v>
+        <v>334</v>
       </c>
       <c r="J18" t="s">
-        <v>340</v>
-      </c>
-      <c r="K18" s="9">
+        <v>335</v>
+      </c>
+      <c r="K18" s="7">
         <v>195</v>
       </c>
     </row>
     <row r="19" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
-        <v>341</v>
+        <v>336</v>
       </c>
       <c r="C19" t="s">
         <v>271</v>
       </c>
       <c r="D19" t="s">
-        <v>342</v>
+        <v>337</v>
       </c>
       <c r="E19">
         <v>0.44</v>
@@ -5454,27 +5736,27 @@
         <v>247</v>
       </c>
       <c r="H19" t="s">
-        <v>343</v>
+        <v>338</v>
       </c>
       <c r="I19" t="s">
-        <v>344</v>
+        <v>339</v>
       </c>
       <c r="J19" t="s">
-        <v>345</v>
-      </c>
-      <c r="K19" s="9">
+        <v>340</v>
+      </c>
+      <c r="K19" s="7">
         <v>295</v>
       </c>
     </row>
     <row r="20" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
-        <v>346</v>
+        <v>341</v>
       </c>
       <c r="C20" t="s">
-        <v>347</v>
+        <v>342</v>
       </c>
       <c r="D20" t="s">
-        <v>348</v>
+        <v>343</v>
       </c>
       <c r="E20">
         <v>7.0000000000000007E-2</v>
@@ -5486,15 +5768,15 @@
         <v>255</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>349</v>
+        <v>344</v>
       </c>
       <c r="I20" s="2" t="s">
-        <v>350</v>
+        <v>345</v>
       </c>
       <c r="J20" t="s">
-        <v>351</v>
-      </c>
-      <c r="K20" s="11">
+        <v>346</v>
+      </c>
+      <c r="K20" s="9">
         <v>59</v>
       </c>
     </row>
@@ -5503,10 +5785,10 @@
         <v>102</v>
       </c>
       <c r="C21" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="D21" t="s">
-        <v>352</v>
+        <v>347</v>
       </c>
       <c r="E21">
         <v>0.7</v>
@@ -5518,27 +5800,27 @@
         <v>255</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>353</v>
+        <v>348</v>
       </c>
       <c r="I21" s="2" t="s">
-        <v>354</v>
+        <v>349</v>
       </c>
       <c r="J21" t="s">
-        <v>355</v>
-      </c>
-      <c r="K21" s="9">
+        <v>350</v>
+      </c>
+      <c r="K21" s="7">
         <v>175</v>
       </c>
     </row>
     <row r="22" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
-        <v>356</v>
+        <v>351</v>
       </c>
       <c r="C22" t="s">
-        <v>357</v>
+        <v>352</v>
       </c>
       <c r="D22" t="s">
-        <v>358</v>
+        <v>353</v>
       </c>
       <c r="E22">
         <v>0.4</v>
@@ -5550,27 +5832,27 @@
         <v>255</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>359</v>
+        <v>354</v>
       </c>
       <c r="I22" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="J22" t="s">
-        <v>360</v>
-      </c>
-      <c r="K22" s="9">
+        <v>355</v>
+      </c>
+      <c r="K22" s="7">
         <v>250</v>
       </c>
     </row>
     <row r="23" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
-        <v>361</v>
+        <v>356</v>
       </c>
       <c r="C23" t="s">
-        <v>362</v>
+        <v>357</v>
       </c>
       <c r="D23" t="s">
-        <v>413</v>
+        <v>407</v>
       </c>
       <c r="E23">
         <v>0.34</v>
@@ -5582,27 +5864,27 @@
         <v>255</v>
       </c>
       <c r="H23" t="s">
-        <v>363</v>
+        <v>358</v>
       </c>
       <c r="I23" t="s">
-        <v>364</v>
+        <v>359</v>
       </c>
       <c r="J23" t="s">
-        <v>365</v>
-      </c>
-      <c r="K23" s="9">
+        <v>360</v>
+      </c>
+      <c r="K23" s="7">
         <v>209</v>
       </c>
     </row>
     <row r="24" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B24" t="s">
-        <v>366</v>
+        <v>361</v>
       </c>
       <c r="C24" t="s">
-        <v>367</v>
+        <v>362</v>
       </c>
       <c r="D24" t="s">
-        <v>368</v>
+        <v>363</v>
       </c>
       <c r="E24">
         <v>0.19</v>
@@ -5613,27 +5895,44 @@
       <c r="G24" t="s">
         <v>255</v>
       </c>
-      <c r="H24" s="18" t="s">
-        <v>407</v>
-      </c>
-      <c r="I24" s="10" t="s">
-        <v>312</v>
+      <c r="H24" s="16" t="s">
+        <v>401</v>
+      </c>
+      <c r="I24" s="8" t="s">
+        <v>309</v>
       </c>
       <c r="J24" t="s">
-        <v>369</v>
-      </c>
-      <c r="K24" s="9">
+        <v>364</v>
+      </c>
+      <c r="K24" s="7">
         <v>265</v>
       </c>
     </row>
     <row r="25" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B25" t="s">
-        <v>370</v>
-      </c>
-      <c r="H25" s="10"/>
-      <c r="I25" s="10"/>
+        <v>365</v>
+      </c>
+      <c r="H25" s="8"/>
+      <c r="I25" s="8"/>
       <c r="J25" t="s">
-        <v>371</v>
+        <v>366</v>
+      </c>
+    </row>
+    <row r="26" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B26" t="s">
+        <v>415</v>
+      </c>
+      <c r="C26" s="19" t="s">
+        <v>416</v>
+      </c>
+      <c r="D26" t="s">
+        <v>417</v>
+      </c>
+      <c r="G26" t="s">
+        <v>255</v>
+      </c>
+      <c r="K26" s="7">
+        <v>189</v>
       </c>
     </row>
   </sheetData>

</xml_diff>